<commit_message>
Added creep roles for Mine/Carry.
</commit_message>
<xml_diff>
--- a/Unit Roles.xlsx
+++ b/Unit Roles.xlsx
@@ -66,10 +66,10 @@
     <t>Badger -&gt; Weasel -&gt; Mongoose</t>
   </si>
   <si>
-    <t>Worm -&gt; Mole -&gt; Rabbit</t>
-  </si>
-  <si>
     <t>Ant -&gt; Beaver -&gt; Termite</t>
+  </si>
+  <si>
+    <t>Mole -&gt; Rabbit -&gt; Elephant</t>
   </si>
 </sst>
 </file>
@@ -473,14 +473,14 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -531,7 +531,7 @@
     </row>
     <row r="5" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -561,7 +561,7 @@
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>

</xml_diff>